<commit_message>
Intentionally ignored file to check GitActions setup
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P097620\Documents\git\user_repos\repo-template-secure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DBE9719-101A-4063-A74A-E97A214E0249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21B4F7A-7446-486F-A134-760C57B8FD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9C75CEBA-89F7-4539-BF59-3D8AE768F7CC}"/>
   </bookViews>
@@ -422,7 +422,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>